<commit_message>
Fully working tracing and outputs without corruption
Fixed the basics, plus also saves part, rev and serial with common code.
Improved initalisation string with instructions too.
</commit_message>
<xml_diff>
--- a/Memory Map.xlsx
+++ b/Memory Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Users\danie\Google Drive\Work\Modbus\Git\ModbusShift\ModbusShift\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338DD389-62AA-4284-B958-BDD54B110543}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F722B461-3ABA-404F-88C5-B3BFCF2304B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{30080191-6877-4434-B289-379CC03641DA}"/>
   </bookViews>
@@ -1172,51 +1172,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1230,6 +1185,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1546,8 +1546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF1C154-DD78-4F44-A5B1-C402DE56878A}">
   <dimension ref="A1:O94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,7 +1608,7 @@
       <c r="B2" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="90" t="s">
+      <c r="C2" s="75" t="s">
         <v>165</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -3005,10 +3005,10 @@
         <v>114</v>
       </c>
       <c r="G37" s="15"/>
-      <c r="H37" s="75" t="s">
+      <c r="H37" s="84" t="s">
         <v>99</v>
       </c>
-      <c r="I37" s="76"/>
+      <c r="I37" s="85"/>
       <c r="J37" s="63"/>
       <c r="K37" s="63"/>
       <c r="L37" s="63"/>
@@ -3019,7 +3019,7 @@
       <c r="A38" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="91" t="s">
+      <c r="B38" s="76" t="s">
         <v>55</v>
       </c>
       <c r="C38" s="26" t="s">
@@ -3037,8 +3037,8 @@
       <c r="G38" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="H38" s="77"/>
-      <c r="I38" s="78"/>
+      <c r="H38" s="86"/>
+      <c r="I38" s="87"/>
       <c r="J38" s="63"/>
       <c r="K38" s="63"/>
       <c r="L38" s="63"/>
@@ -3052,7 +3052,7 @@
       <c r="B39" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="95">
+      <c r="C39" s="80">
         <v>256</v>
       </c>
       <c r="D39" s="29" t="s">
@@ -3061,7 +3061,7 @@
       <c r="E39" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="F39" s="85" t="s">
+      <c r="F39" s="94" t="s">
         <v>163</v>
       </c>
       <c r="G39" s="9" t="s">
@@ -3086,7 +3086,7 @@
       <c r="B40" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="96">
+      <c r="C40" s="81">
         <v>257</v>
       </c>
       <c r="D40" s="31" t="s">
@@ -3095,7 +3095,7 @@
       <c r="E40" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="F40" s="86"/>
+      <c r="F40" s="95"/>
       <c r="G40" s="4" t="s">
         <v>36</v>
       </c>
@@ -3118,7 +3118,7 @@
       <c r="B41" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="96">
+      <c r="C41" s="81">
         <v>258</v>
       </c>
       <c r="D41" s="31" t="s">
@@ -3127,7 +3127,7 @@
       <c r="E41" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="F41" s="86"/>
+      <c r="F41" s="95"/>
       <c r="G41" s="4" t="s">
         <v>36</v>
       </c>
@@ -3150,7 +3150,7 @@
       <c r="B42" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="97">
+      <c r="C42" s="82">
         <v>259</v>
       </c>
       <c r="D42" s="31" t="s">
@@ -3159,7 +3159,7 @@
       <c r="E42" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="F42" s="86"/>
+      <c r="F42" s="95"/>
       <c r="G42" s="4" t="s">
         <v>36</v>
       </c>
@@ -3182,7 +3182,7 @@
       <c r="B43" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C43" s="97">
+      <c r="C43" s="82">
         <v>260</v>
       </c>
       <c r="D43" s="31" t="s">
@@ -3191,7 +3191,7 @@
       <c r="E43" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="F43" s="86"/>
+      <c r="F43" s="95"/>
       <c r="G43" s="4" t="s">
         <v>36</v>
       </c>
@@ -3214,7 +3214,7 @@
       <c r="B44" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="97">
+      <c r="C44" s="82">
         <v>261</v>
       </c>
       <c r="D44" s="31" t="s">
@@ -3223,7 +3223,7 @@
       <c r="E44" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="F44" s="86"/>
+      <c r="F44" s="95"/>
       <c r="G44" s="4" t="s">
         <v>36</v>
       </c>
@@ -3246,7 +3246,7 @@
       <c r="B45" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C45" s="97">
+      <c r="C45" s="82">
         <v>262</v>
       </c>
       <c r="D45" s="31" t="s">
@@ -3255,7 +3255,7 @@
       <c r="E45" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="F45" s="86"/>
+      <c r="F45" s="95"/>
       <c r="G45" s="4" t="s">
         <v>36</v>
       </c>
@@ -3278,7 +3278,7 @@
       <c r="B46" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C46" s="97">
+      <c r="C46" s="82">
         <v>263</v>
       </c>
       <c r="D46" s="31" t="s">
@@ -3287,7 +3287,7 @@
       <c r="E46" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="F46" s="86"/>
+      <c r="F46" s="95"/>
       <c r="G46" s="4" t="s">
         <v>36</v>
       </c>
@@ -3310,7 +3310,7 @@
       <c r="B47" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="C47" s="98">
+      <c r="C47" s="83">
         <v>264</v>
       </c>
       <c r="D47" s="50" t="s">
@@ -3319,7 +3319,7 @@
       <c r="E47" s="51" t="s">
         <v>98</v>
       </c>
-      <c r="F47" s="87"/>
+      <c r="F47" s="96"/>
       <c r="G47" s="23" t="s">
         <v>36</v>
       </c>
@@ -3378,10 +3378,10 @@
         <v>115</v>
       </c>
       <c r="G50" s="15"/>
-      <c r="H50" s="75" t="s">
+      <c r="H50" s="84" t="s">
         <v>99</v>
       </c>
-      <c r="I50" s="76"/>
+      <c r="I50" s="85"/>
       <c r="J50" s="63"/>
       <c r="K50" s="63"/>
       <c r="L50" s="63"/>
@@ -3395,7 +3395,7 @@
       <c r="B51" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C51" s="90" t="s">
+      <c r="C51" s="75" t="s">
         <v>165</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -3410,8 +3410,8 @@
       <c r="G51" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H51" s="82"/>
-      <c r="I51" s="78"/>
+      <c r="H51" s="91"/>
+      <c r="I51" s="87"/>
       <c r="J51" s="63"/>
       <c r="K51" s="63"/>
       <c r="L51" s="63"/>
@@ -3425,7 +3425,7 @@
       <c r="B52" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="C52" s="92">
+      <c r="C52" s="77">
         <v>512</v>
       </c>
       <c r="D52" s="59" t="s">
@@ -3479,10 +3479,10 @@
         <v>116</v>
       </c>
       <c r="G54" s="15"/>
-      <c r="H54" s="75" t="s">
+      <c r="H54" s="84" t="s">
         <v>99</v>
       </c>
-      <c r="I54" s="76"/>
+      <c r="I54" s="85"/>
       <c r="J54" s="63"/>
       <c r="K54" s="63"/>
       <c r="L54" s="63"/>
@@ -3496,7 +3496,7 @@
       <c r="B55" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C55" s="90" t="s">
+      <c r="C55" s="75" t="s">
         <v>165</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -3511,8 +3511,8 @@
       <c r="G55" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H55" s="83"/>
-      <c r="I55" s="84"/>
+      <c r="H55" s="92"/>
+      <c r="I55" s="93"/>
       <c r="J55" s="63"/>
       <c r="K55" s="63"/>
       <c r="L55" s="63"/>
@@ -3535,7 +3535,7 @@
       <c r="E56" s="30">
         <v>1</v>
       </c>
-      <c r="F56" s="85" t="s">
+      <c r="F56" s="94" t="s">
         <v>164</v>
       </c>
       <c r="G56" s="38" t="s">
@@ -3569,7 +3569,7 @@
       <c r="E57" s="32">
         <v>9</v>
       </c>
-      <c r="F57" s="86"/>
+      <c r="F57" s="95"/>
       <c r="G57" s="10" t="s">
         <v>36</v>
       </c>
@@ -3601,7 +3601,7 @@
       <c r="E58" s="32">
         <v>0</v>
       </c>
-      <c r="F58" s="86"/>
+      <c r="F58" s="95"/>
       <c r="G58" s="10" t="s">
         <v>36</v>
       </c>
@@ -3633,7 +3633,7 @@
       <c r="E59" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="F59" s="86"/>
+      <c r="F59" s="95"/>
       <c r="G59" s="10" t="s">
         <v>36</v>
       </c>
@@ -3665,7 +3665,7 @@
       <c r="E60" s="51" t="s">
         <v>98</v>
       </c>
-      <c r="F60" s="87"/>
+      <c r="F60" s="96"/>
       <c r="G60" s="55" t="s">
         <v>36</v>
       </c>
@@ -3708,10 +3708,10 @@
         <v>117</v>
       </c>
       <c r="G62" s="15"/>
-      <c r="H62" s="75" t="s">
+      <c r="H62" s="84" t="s">
         <v>99</v>
       </c>
-      <c r="I62" s="76"/>
+      <c r="I62" s="85"/>
       <c r="J62" s="63"/>
       <c r="K62" s="63"/>
       <c r="L62" s="63"/>
@@ -3725,7 +3725,7 @@
       <c r="B63" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C63" s="90" t="s">
+      <c r="C63" s="75" t="s">
         <v>165</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -3740,8 +3740,8 @@
       <c r="G63" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H63" s="82"/>
-      <c r="I63" s="78"/>
+      <c r="H63" s="91"/>
+      <c r="I63" s="87"/>
       <c r="J63" s="63"/>
       <c r="K63" s="63"/>
       <c r="L63" s="63"/>
@@ -3764,7 +3764,7 @@
       <c r="E64" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="F64" s="79" t="s">
+      <c r="F64" s="88" t="s">
         <v>83</v>
       </c>
       <c r="G64" s="38" t="s">
@@ -3798,7 +3798,7 @@
       <c r="E65" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="F65" s="80"/>
+      <c r="F65" s="89"/>
       <c r="G65" s="11" t="s">
         <v>36</v>
       </c>
@@ -3830,7 +3830,7 @@
       <c r="E66" s="32">
         <v>9</v>
       </c>
-      <c r="F66" s="80"/>
+      <c r="F66" s="89"/>
       <c r="G66" s="11" t="s">
         <v>36</v>
       </c>
@@ -3862,7 +3862,7 @@
       <c r="E67" s="32">
         <v>0</v>
       </c>
-      <c r="F67" s="80"/>
+      <c r="F67" s="89"/>
       <c r="G67" s="11" t="s">
         <v>36</v>
       </c>
@@ -3894,7 +3894,7 @@
       <c r="E68" s="51">
         <v>1</v>
       </c>
-      <c r="F68" s="81"/>
+      <c r="F68" s="90"/>
       <c r="G68" s="55" t="s">
         <v>36</v>
       </c>
@@ -3937,10 +3937,10 @@
         <v>118</v>
       </c>
       <c r="G70" s="15"/>
-      <c r="H70" s="75" t="s">
+      <c r="H70" s="84" t="s">
         <v>99</v>
       </c>
-      <c r="I70" s="76"/>
+      <c r="I70" s="85"/>
       <c r="J70" s="63"/>
       <c r="K70" s="63"/>
       <c r="L70" s="63"/>
@@ -3954,7 +3954,7 @@
       <c r="B71" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C71" s="90" t="s">
+      <c r="C71" s="75" t="s">
         <v>165</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -3969,8 +3969,8 @@
       <c r="G71" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H71" s="82"/>
-      <c r="I71" s="78"/>
+      <c r="H71" s="91"/>
+      <c r="I71" s="87"/>
       <c r="J71" s="63"/>
       <c r="K71" s="63"/>
       <c r="L71" s="63"/>
@@ -3982,7 +3982,7 @@
         <v>42</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C72" s="6">
         <v>1280</v>
@@ -3993,7 +3993,7 @@
       <c r="E72" s="30">
         <v>7</v>
       </c>
-      <c r="F72" s="79" t="s">
+      <c r="F72" s="88" t="s">
         <v>82</v>
       </c>
       <c r="G72" s="38" t="s">
@@ -4016,7 +4016,7 @@
         <v>42</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C73" s="10">
         <v>1281</v>
@@ -4027,7 +4027,7 @@
       <c r="E73" s="32">
         <v>5</v>
       </c>
-      <c r="F73" s="80"/>
+      <c r="F73" s="89"/>
       <c r="G73" s="11" t="s">
         <v>36</v>
       </c>
@@ -4048,7 +4048,7 @@
         <v>42</v>
       </c>
       <c r="B74" s="23" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C74" s="20">
         <v>1282</v>
@@ -4059,7 +4059,7 @@
       <c r="E74" s="51">
         <v>9</v>
       </c>
-      <c r="F74" s="81"/>
+      <c r="F74" s="90"/>
       <c r="G74" s="55" t="s">
         <v>36</v>
       </c>
@@ -4102,10 +4102,10 @@
         <v>119</v>
       </c>
       <c r="G76" s="15"/>
-      <c r="H76" s="75" t="s">
+      <c r="H76" s="84" t="s">
         <v>99</v>
       </c>
-      <c r="I76" s="76"/>
+      <c r="I76" s="85"/>
       <c r="J76" s="63"/>
       <c r="K76" s="63"/>
       <c r="L76" s="63"/>
@@ -4119,7 +4119,7 @@
       <c r="B77" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C77" s="90" t="s">
+      <c r="C77" s="75" t="s">
         <v>165</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -4134,8 +4134,8 @@
       <c r="G77" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H77" s="82"/>
-      <c r="I77" s="78"/>
+      <c r="H77" s="91"/>
+      <c r="I77" s="87"/>
       <c r="J77" s="63"/>
       <c r="K77" s="63"/>
       <c r="L77" s="63"/>
@@ -4158,7 +4158,7 @@
       <c r="E78" s="30">
         <v>1</v>
       </c>
-      <c r="F78" s="88" t="s">
+      <c r="F78" s="97" t="s">
         <v>84</v>
       </c>
       <c r="G78" s="38" t="s">
@@ -4192,7 +4192,7 @@
       <c r="E79" s="51">
         <v>0</v>
       </c>
-      <c r="F79" s="89"/>
+      <c r="F79" s="98"/>
       <c r="G79" s="55" t="s">
         <v>36</v>
       </c>
@@ -4235,10 +4235,10 @@
         <v>120</v>
       </c>
       <c r="G81" s="15"/>
-      <c r="H81" s="75" t="s">
+      <c r="H81" s="84" t="s">
         <v>99</v>
       </c>
-      <c r="I81" s="76"/>
+      <c r="I81" s="85"/>
       <c r="J81" s="63"/>
       <c r="K81" s="63"/>
       <c r="L81" s="63"/>
@@ -4252,7 +4252,7 @@
       <c r="B82" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C82" s="90" t="s">
+      <c r="C82" s="75" t="s">
         <v>165</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -4267,8 +4267,8 @@
       <c r="G82" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H82" s="82"/>
-      <c r="I82" s="78"/>
+      <c r="H82" s="91"/>
+      <c r="I82" s="87"/>
       <c r="J82" s="63"/>
       <c r="K82" s="63"/>
       <c r="L82" s="63"/>
@@ -4282,7 +4282,7 @@
       <c r="B83" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="C83" s="93">
+      <c r="C83" s="78">
         <v>1792</v>
       </c>
       <c r="D83" s="35" t="s">
@@ -4316,7 +4316,7 @@
       <c r="B84" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C84" s="94">
+      <c r="C84" s="79">
         <v>1793</v>
       </c>
       <c r="D84" s="33" t="s">
@@ -4350,7 +4350,7 @@
       <c r="B85" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="C85" s="92">
+      <c r="C85" s="77">
         <v>1794</v>
       </c>
       <c r="D85" s="59" t="s">

</xml_diff>

<commit_message>
Improved description of Modbus response when PrintF
Added byte descriptions on the Modbus response Printf function.
</commit_message>
<xml_diff>
--- a/Memory Map.xlsx
+++ b/Memory Map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Users\danie\Google Drive\Work\Modbus\Git\ModbusShift\ModbusShift\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50163D20-06D0-4D62-9BAF-16E956DBB653}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBBD2F0-3B63-43FA-9951-9BFEF9FCE35B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32670" yWindow="705" windowWidth="20145" windowHeight="20640" xr2:uid="{30080191-6877-4434-B289-379CC03641DA}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{30080191-6877-4434-B289-379CC03641DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="167">
   <si>
     <t>MB300xx</t>
   </si>
@@ -536,6 +536,9 @@
   </si>
   <si>
     <t>0x0605</t>
+  </si>
+  <si>
+    <t>(0xFF)</t>
   </si>
 </sst>
 </file>
@@ -1553,8 +1556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF1C154-DD78-4F44-A5B1-C402DE56878A}">
   <dimension ref="A1:N85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="V52" sqref="V52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3505,7 +3508,7 @@
         <v>1</v>
       </c>
       <c r="E59" s="39" t="s">
-        <v>92</v>
+        <v>166</v>
       </c>
       <c r="F59" s="89"/>
       <c r="G59" s="17" t="s">
@@ -3529,10 +3532,10 @@
         <v>772</v>
       </c>
       <c r="D60" s="42" t="s">
-        <v>92</v>
+        <v>166</v>
       </c>
       <c r="E60" s="43" t="s">
-        <v>92</v>
+        <v>166</v>
       </c>
       <c r="F60" s="90"/>
       <c r="G60" s="22" t="s">
@@ -3828,7 +3831,7 @@
         <v>42</v>
       </c>
       <c r="B73" s="35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C73" s="31">
         <v>1280</v>
@@ -3857,7 +3860,7 @@
         <v>42</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C74" s="17">
         <v>1281</v>
@@ -3884,7 +3887,7 @@
         <v>42</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C75" s="17">
         <v>1282</v>
@@ -3911,7 +3914,7 @@
         <v>42</v>
       </c>
       <c r="B76" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C76" s="22">
         <v>1283</v>

</xml_diff>